<commit_message>
starting to validate using multiple segmentations
</commit_message>
<xml_diff>
--- a/figs/PVE_active_contours.xlsx
+++ b/figs/PVE_active_contours.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="46">
   <si>
     <t xml:space="preserve">Edges</t>
   </si>
@@ -157,10 +157,10 @@
     <t xml:space="preserve">Snakes – 2412-01</t>
   </si>
   <si>
-    <t xml:space="preserve">Snakes – 040118</t>
+    <t xml:space="preserve">Snakes – 080118</t>
   </si>
   <si>
-    <t xml:space="preserve">Snakes – 080118</t>
+    <t xml:space="preserve">Snakes – 040118</t>
   </si>
 </sst>
 </file>
@@ -3122,7 +3122,7 @@
   <dimension ref="A1:Z46"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4663,10 +4663,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4703,6 +4703,33 @@
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z1" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -4735,36 +4762,96 @@
         <f aca="false">MIN(B2:F2)</f>
         <v>22822.453</v>
       </c>
+      <c r="R2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="S2" s="2" t="n">
+        <v>52295.681</v>
+      </c>
+      <c r="T2" s="2" t="n">
+        <v>25264.893</v>
+      </c>
+      <c r="U2" s="2" t="n">
+        <v>22822.453</v>
+      </c>
+      <c r="V2" s="2" t="n">
+        <v>25799.604</v>
+      </c>
+      <c r="W2" s="2" t="n">
+        <v>50882.94</v>
+      </c>
+      <c r="X2" s="0" t="n">
+        <f aca="false">AVERAGE(S2:W2)</f>
+        <v>35413.1142</v>
+      </c>
+      <c r="Y2" s="0" t="n">
+        <f aca="false">MAX(S2:W2)</f>
+        <v>52295.681</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <f aca="false">MIN(S2:W2)</f>
+        <v>22822.453</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>47610.955</v>
+        <v>50489.041</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>25605.469</v>
+        <v>26636.353</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>21790.472</v>
+        <v>22447.735</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>24998.141</v>
+        <v>25309.994</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>47615.576</v>
+        <v>48363.256</v>
       </c>
       <c r="G3" s="0" t="n">
         <f aca="false">AVERAGE(B3:F3)</f>
-        <v>33524.1226</v>
+        <v>34649.2758</v>
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">MAX(B3:F3)</f>
-        <v>47615.576</v>
+        <v>50489.041</v>
       </c>
       <c r="I3" s="0" t="n">
         <f aca="false">MIN(B3:F3)</f>
+        <v>22447.735</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="S3" s="2" t="n">
+        <v>47610.955</v>
+      </c>
+      <c r="T3" s="2" t="n">
+        <v>25605.469</v>
+      </c>
+      <c r="U3" s="2" t="n">
+        <v>21790.472</v>
+      </c>
+      <c r="V3" s="2" t="n">
+        <v>24998.141</v>
+      </c>
+      <c r="W3" s="2" t="n">
+        <v>47615.576</v>
+      </c>
+      <c r="X3" s="0" t="n">
+        <f aca="false">AVERAGE(S3:W3)</f>
+        <v>33524.1226</v>
+      </c>
+      <c r="Y3" s="0" t="n">
+        <f aca="false">MAX(S3:W3)</f>
+        <v>47615.576</v>
+      </c>
+      <c r="Z3" s="0" t="n">
+        <f aca="false">MIN(S3:W3)</f>
         <v>21790.472</v>
       </c>
     </row>
@@ -4773,30 +4860,60 @@
         <v>12</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.09</v>
+        <v>0.035</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>-0.013</v>
+        <v>-0.054</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.045</v>
+        <v>0.016</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.031</v>
+        <v>0.019</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>0.064</v>
-      </c>
-      <c r="G4" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="G4" s="9" t="n">
         <f aca="false">AVERAGE(B4:F4)</f>
-        <v>0.0434</v>
+        <v>0.0132</v>
       </c>
       <c r="H4" s="3" t="n">
         <f aca="false">MAX(B4:F4)</f>
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="I4" s="3" t="n">
         <f aca="false">MIN(B4:F4)</f>
+        <v>-0.054</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="T4" s="3" t="n">
+        <v>-0.013</v>
+      </c>
+      <c r="U4" s="3" t="n">
+        <v>0.045</v>
+      </c>
+      <c r="V4" s="3" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="W4" s="3" t="n">
+        <v>0.064</v>
+      </c>
+      <c r="X4" s="3" t="n">
+        <f aca="false">AVERAGE(S4:W4)</f>
+        <v>0.0434</v>
+      </c>
+      <c r="Y4" s="3" t="n">
+        <f aca="false">MAX(S4:W4)</f>
+        <v>0.09</v>
+      </c>
+      <c r="Z4" s="3" t="n">
+        <f aca="false">MIN(S4:W4)</f>
         <v>-0.013</v>
       </c>
     </row>
@@ -4831,36 +4948,96 @@
         <f aca="false">MIN(B5:F5)</f>
         <v>9591.064</v>
       </c>
+      <c r="R5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>32805.908</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>9591.064</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>11771.3</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>15589.534</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>34140.034</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <f aca="false">AVERAGE(S5:W5)</f>
+        <v>20779.568</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <f aca="false">MAX(S5:W5)</f>
+        <v>34140.034</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <f aca="false">MIN(S5:W5)</f>
+        <v>9591.064</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>28119.757</v>
+        <v>31002.118</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>10344.238</v>
+        <v>10946.655</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>10443.852</v>
+        <v>11019.281</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>14772.479</v>
+        <v>15103.044</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>34042.368</v>
+        <v>34800.329</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">AVERAGE(B6:F6)</f>
-        <v>19544.5388</v>
+        <v>20574.2854</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">MAX(B6:F6)</f>
-        <v>34042.368</v>
+        <v>34800.329</v>
       </c>
       <c r="I6" s="0" t="n">
         <f aca="false">MIN(B6:F6)</f>
+        <v>10946.655</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="S6" s="2" t="n">
+        <v>28119.757</v>
+      </c>
+      <c r="T6" s="2" t="n">
+        <v>10344.238</v>
+      </c>
+      <c r="U6" s="2" t="n">
+        <v>10443.852</v>
+      </c>
+      <c r="V6" s="2" t="n">
+        <v>14772.479</v>
+      </c>
+      <c r="W6" s="2" t="n">
+        <v>34042.368</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <f aca="false">AVERAGE(S6:W6)</f>
+        <v>19544.5388</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <f aca="false">MAX(S6:W6)</f>
+        <v>34042.368</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <f aca="false">MIN(S6:W6)</f>
         <v>10344.238</v>
       </c>
     </row>
@@ -4868,31 +5045,61 @@
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>0.143</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>-0.079</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>0.113</v>
+      <c r="B7" s="3" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>-0.141</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0.064</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.052</v>
+        <v>0.031</v>
       </c>
       <c r="F7" s="3" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="G7" s="3" t="n">
+        <v>-0.019</v>
+      </c>
+      <c r="G7" s="9" t="n">
         <f aca="false">AVERAGE(B7:F7)</f>
-        <v>0.0464</v>
+        <v>-0.002</v>
       </c>
       <c r="H7" s="3" t="n">
         <f aca="false">MAX(B7:F7)</f>
-        <v>0.143</v>
+        <v>0.064</v>
       </c>
       <c r="I7" s="3" t="n">
         <f aca="false">MIN(B7:F7)</f>
+        <v>-0.141</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S7" s="4" t="n">
+        <v>0.143</v>
+      </c>
+      <c r="T7" s="3" t="n">
+        <v>-0.079</v>
+      </c>
+      <c r="U7" s="4" t="n">
+        <v>0.113</v>
+      </c>
+      <c r="V7" s="3" t="n">
+        <v>0.052</v>
+      </c>
+      <c r="W7" s="3" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="X7" s="3" t="n">
+        <f aca="false">AVERAGE(S7:W7)</f>
+        <v>0.0464</v>
+      </c>
+      <c r="Y7" s="3" t="n">
+        <f aca="false">MAX(S7:W7)</f>
+        <v>0.143</v>
+      </c>
+      <c r="Z7" s="3" t="n">
+        <f aca="false">MIN(S7:W7)</f>
         <v>-0.079</v>
       </c>
     </row>
@@ -4927,36 +5134,96 @@
         <f aca="false">MIN(B8:F8)</f>
         <v>10210.069</v>
       </c>
+      <c r="R8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="S8" s="2" t="n">
+        <v>19489.773</v>
+      </c>
+      <c r="T8" s="2" t="n">
+        <v>15673.828</v>
+      </c>
+      <c r="U8" s="2" t="n">
+        <v>11051.153</v>
+      </c>
+      <c r="V8" s="2" t="n">
+        <v>10210.069</v>
+      </c>
+      <c r="W8" s="2" t="n">
+        <v>16742.907</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <f aca="false">AVERAGE(S8:W8)</f>
+        <v>14633.546</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <f aca="false">MAX(S8:W8)</f>
+        <v>19489.773</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <f aca="false">MIN(S8:W8)</f>
+        <v>10210.069</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>19491.198</v>
+        <v>19486.923</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>15261.23</v>
+        <v>15689.697</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>11346.62</v>
+        <v>11428.455</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>10225.662</v>
+        <v>10206.951</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>13573.208</v>
+        <v>13562.927</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">AVERAGE(B9:F9)</f>
-        <v>13979.5836</v>
+        <v>14074.9906</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">MAX(B9:F9)</f>
-        <v>19491.198</v>
+        <v>19486.923</v>
       </c>
       <c r="I9" s="0" t="n">
         <f aca="false">MIN(B9:F9)</f>
+        <v>10206.951</v>
+      </c>
+      <c r="R9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S9" s="2" t="n">
+        <v>19491.198</v>
+      </c>
+      <c r="T9" s="2" t="n">
+        <v>15261.23</v>
+      </c>
+      <c r="U9" s="2" t="n">
+        <v>11346.62</v>
+      </c>
+      <c r="V9" s="2" t="n">
+        <v>10225.662</v>
+      </c>
+      <c r="W9" s="2" t="n">
+        <v>13573.208</v>
+      </c>
+      <c r="X9" s="0" t="n">
+        <f aca="false">AVERAGE(S9:W9)</f>
+        <v>13979.5836</v>
+      </c>
+      <c r="Y9" s="0" t="n">
+        <f aca="false">MAX(S9:W9)</f>
+        <v>19491.198</v>
+      </c>
+      <c r="Z9" s="0" t="n">
+        <f aca="false">MIN(S9:W9)</f>
         <v>10225.662</v>
       </c>
     </row>
@@ -4968,57 +5235,84 @@
         <v>0</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.026</v>
+        <v>-0.001</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>-0.027</v>
+        <v>-0.034</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>-0.002</v>
+        <v>0</v>
       </c>
       <c r="F10" s="4" t="n">
-        <v>0.189</v>
+        <v>0.19</v>
       </c>
       <c r="G10" s="9" t="n">
         <f aca="false">AVERAGE(B10:F10)</f>
-        <v>0.0372</v>
+        <v>0.031</v>
       </c>
       <c r="H10" s="3" t="n">
         <f aca="false">MAX(B10:F10)</f>
-        <v>0.189</v>
+        <v>0.19</v>
       </c>
       <c r="I10" s="3" t="n">
         <f aca="false">MIN(B10:F10)</f>
+        <v>-0.034</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="T10" s="3" t="n">
+        <v>0.026</v>
+      </c>
+      <c r="U10" s="3" t="n">
         <v>-0.027</v>
       </c>
+      <c r="V10" s="3" t="n">
+        <v>-0.002</v>
+      </c>
+      <c r="W10" s="4" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="X10" s="9" t="n">
+        <f aca="false">AVERAGE(S10:W10)</f>
+        <v>0.0372</v>
+      </c>
+      <c r="Y10" s="3" t="n">
+        <f aca="false">MAX(S10:W10)</f>
+        <v>0.189</v>
+      </c>
+      <c r="Z10" s="3" t="n">
+        <f aca="false">MIN(S10:W10)</f>
+        <v>-0.027</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="B13" s="0" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5026,31 +5320,31 @@
         <v>10</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>52295.681</v>
+        <v>120906.532</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>25264.893</v>
+        <v>7491.171</v>
       </c>
       <c r="D14" s="2" t="n">
-        <v>22822.453</v>
+        <v>46110.674</v>
       </c>
       <c r="E14" s="2" t="n">
-        <v>25799.604</v>
+        <v>20431.929</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>50882.94</v>
+        <v>36392.609</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">AVERAGE(B14:F14)</f>
-        <v>35413.1142</v>
+        <v>46266.583</v>
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">MAX(B14:F14)</f>
-        <v>52295.681</v>
+        <v>120906.532</v>
       </c>
       <c r="I14" s="0" t="n">
         <f aca="false">MIN(B14:F14)</f>
-        <v>22822.453</v>
+        <v>7491.171</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5058,31 +5352,31 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="n">
-        <v>50489.041</v>
+        <v>129247.624</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>26636.353</v>
+        <v>7904.415</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>22447.735</v>
+        <v>42328.274</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>25309.994</v>
+        <v>21630.202</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>48363.256</v>
+        <v>40096.161</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">AVERAGE(B15:F15)</f>
-        <v>34649.2758</v>
+        <v>48241.3352</v>
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">MAX(B15:F15)</f>
-        <v>50489.041</v>
+        <v>129247.624</v>
       </c>
       <c r="I15" s="0" t="n">
         <f aca="false">MIN(B15:F15)</f>
-        <v>22447.735</v>
+        <v>7904.415</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5090,63 +5384,64 @@
         <v>12</v>
       </c>
       <c r="B16" s="3" t="n">
-        <v>0.035</v>
+        <v>-0.069</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>-0.054</v>
+        <v>-0.055</v>
       </c>
       <c r="D16" s="3" t="n">
-        <v>0.016</v>
+        <v>0.082</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>0.019</v>
-      </c>
-      <c r="F16" s="3" t="n">
-        <v>0.05</v>
+        <f aca="false">-0.059</f>
+        <v>-0.059</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>-0.102</v>
       </c>
       <c r="G16" s="9" t="n">
         <f aca="false">AVERAGE(B16:F16)</f>
-        <v>0.0132</v>
+        <v>-0.0406</v>
       </c>
       <c r="H16" s="3" t="n">
         <f aca="false">MAX(B16:F16)</f>
-        <v>0.05</v>
+        <v>0.082</v>
       </c>
       <c r="I16" s="3" t="n">
         <f aca="false">MIN(B16:F16)</f>
-        <v>-0.054</v>
+        <v>-0.102</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="0" t="n">
-        <v>32805.908</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>9591.064</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>11771.3</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>15589.534</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>34140.034</v>
+      <c r="B17" s="2" t="n">
+        <v>87365.054</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>4787.118</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>25932.182</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>13412.84</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>21954.762</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">AVERAGE(B17:F17)</f>
-        <v>20779.568</v>
+        <v>30690.3912</v>
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">MAX(B17:F17)</f>
-        <v>34140.034</v>
+        <v>87365.054</v>
       </c>
       <c r="I17" s="0" t="n">
         <f aca="false">MIN(B17:F17)</f>
-        <v>9591.064</v>
+        <v>4787.118</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5154,63 +5449,63 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="n">
-        <v>31002.118</v>
+        <v>98700.103</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>10946.655</v>
+        <v>5199.239</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>11019.281</v>
+        <v>29723.124</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>15103.044</v>
+        <v>12423.309</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>34800.329</v>
+        <v>25676.147</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">AVERAGE(B18:F18)</f>
-        <v>20574.2854</v>
+        <v>34344.3844</v>
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">MAX(B18:F18)</f>
-        <v>34800.329</v>
+        <v>98700.103</v>
       </c>
       <c r="I18" s="0" t="n">
         <f aca="false">MIN(B18:F18)</f>
-        <v>10946.655</v>
+        <v>5199.239</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="3" t="n">
-        <v>0.055</v>
-      </c>
-      <c r="C19" s="4" t="n">
-        <v>-0.141</v>
-      </c>
-      <c r="D19" s="3" t="n">
-        <v>0.064</v>
+      <c r="B19" s="4" t="n">
+        <v>-0.13</v>
+      </c>
+      <c r="C19" s="3" t="n">
+        <v>-0.086</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>-0.146</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>0.031</v>
-      </c>
-      <c r="F19" s="3" t="n">
-        <v>-0.019</v>
+        <v>0.074</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <v>-0.17</v>
       </c>
       <c r="G19" s="9" t="n">
         <f aca="false">AVERAGE(B19:F19)</f>
-        <v>-0.002</v>
+        <v>-0.0916</v>
       </c>
       <c r="H19" s="3" t="n">
         <f aca="false">MAX(B19:F19)</f>
-        <v>0.064</v>
+        <v>0.074</v>
       </c>
       <c r="I19" s="3" t="n">
         <f aca="false">MIN(B19:F19)</f>
-        <v>-0.141</v>
+        <v>-0.17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5218,31 +5513,31 @@
         <v>16</v>
       </c>
       <c r="B20" s="2" t="n">
-        <v>19489.773</v>
+        <v>33541.478</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>15673.828</v>
+        <v>2704.053</v>
       </c>
       <c r="D20" s="2" t="n">
-        <v>11051.153</v>
+        <v>20178.492</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>10210.069</v>
+        <v>7019.09</v>
       </c>
       <c r="F20" s="2" t="n">
-        <v>16742.907</v>
+        <v>14437.847</v>
       </c>
       <c r="G20" s="0" t="n">
         <f aca="false">AVERAGE(B20:F20)</f>
-        <v>14633.546</v>
+        <v>15576.192</v>
       </c>
       <c r="H20" s="0" t="n">
         <f aca="false">MAX(B20:F20)</f>
-        <v>19489.773</v>
+        <v>33541.478</v>
       </c>
       <c r="I20" s="0" t="n">
         <f aca="false">MIN(B20:F20)</f>
-        <v>10210.069</v>
+        <v>2704.053</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5250,31 +5545,31 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="n">
-        <v>19486.923</v>
+        <v>30547.521</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>15689.697</v>
+        <v>2705.176</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>11428.455</v>
+        <v>12605.15</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>10206.951</v>
+        <v>9206.893</v>
       </c>
       <c r="F21" s="2" t="n">
-        <v>13562.927</v>
+        <v>14420.014</v>
       </c>
       <c r="G21" s="0" t="n">
         <f aca="false">AVERAGE(B21:F21)</f>
-        <v>14074.9906</v>
+        <v>13896.9508</v>
       </c>
       <c r="H21" s="0" t="n">
         <f aca="false">MAX(B21:F21)</f>
-        <v>19486.923</v>
+        <v>30547.521</v>
       </c>
       <c r="I21" s="0" t="n">
         <f aca="false">MIN(B21:F21)</f>
-        <v>10206.951</v>
+        <v>2705.176</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5282,31 +5577,31 @@
         <v>18</v>
       </c>
       <c r="B22" s="3" t="n">
+        <v>0.089</v>
+      </c>
+      <c r="C22" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="3" t="n">
-        <v>-0.001</v>
-      </c>
-      <c r="D22" s="3" t="n">
-        <v>-0.034</v>
-      </c>
-      <c r="E22" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4" t="n">
-        <v>0.19</v>
+      <c r="D22" s="4" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>-0.312</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0.001</v>
       </c>
       <c r="G22" s="9" t="n">
         <f aca="false">AVERAGE(B22:F22)</f>
-        <v>0.031</v>
+        <v>0.0306</v>
       </c>
       <c r="H22" s="3" t="n">
         <f aca="false">MAX(B22:F22)</f>
-        <v>0.19</v>
+        <v>0.375</v>
       </c>
       <c r="I22" s="3" t="n">
         <f aca="false">MIN(B22:F22)</f>
-        <v>-0.034</v>
+        <v>-0.312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commiting before rethinking the project
</commit_message>
<xml_diff>
--- a/figs/PVE_active_contours.xlsx
+++ b/figs/PVE_active_contours.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="47">
   <si>
     <t xml:space="preserve">Edges</t>
   </si>
@@ -161,6 +162,9 @@
   </si>
   <si>
     <t xml:space="preserve">Snakes – 040118</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Edges – Feb18</t>
   </si>
 </sst>
 </file>
@@ -386,14 +390,14 @@
   </sheetPr>
   <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.015306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.8724489795918"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="54.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2618,7 +2622,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -2633,14 +2637,14 @@
   </sheetPr>
   <dimension ref="A1:AK11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="55.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.8724489795918"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="55.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +3110,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3121,14 +3125,14 @@
   </sheetPr>
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6275510204082"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4650,7 +4654,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4665,14 +4669,14 @@
   </sheetPr>
   <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.6530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.6275510204082"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5607,7 +5611,1236 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J46"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I56" activeCellId="0" sqref="I56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="52.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>52295.681</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>25264.893</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>22822.453</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>25799.604</v>
+      </c>
+      <c r="F2" s="2" t="n">
+        <v>50882.94</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <f aca="false">AVERAGE(B2:F2)</f>
+        <v>35413.1142</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <f aca="false">MAX(B2:F2)</f>
+        <v>52295.681</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <f aca="false">MIN(B2:F2)</f>
+        <v>22822.453</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>50818.169</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>23499.146</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>21317.553</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>26544.932</v>
+      </c>
+      <c r="F3" s="2" t="n">
+        <v>49375.896</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <f aca="false">AVERAGE(B3:F3)</f>
+        <v>34311.1392</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <f aca="false">MAX(B3:F3)</f>
+        <v>50818.169</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <f aca="false">MIN(B3:F3)</f>
+        <v>21317.553</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.028</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0.066</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>-0.029</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <f aca="false">AVERAGE(B4:F4)</f>
+        <v>0.033</v>
+      </c>
+      <c r="H4" s="3" t="n">
+        <f aca="false">MAX(B4:F4)</f>
+        <v>0.07</v>
+      </c>
+      <c r="I4" s="3" t="n">
+        <f aca="false">MIN(B4:F4)</f>
+        <v>-0.029</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>32805.908</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9591.064</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>11771.3</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>15589.534</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>34140.034</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <f aca="false">AVERAGE(B5:F5)</f>
+        <v>20779.568</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <f aca="false">MAX(B5:F5)</f>
+        <v>34140.034</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">MIN(B5:F5)</f>
+        <v>9591.064</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>30493.466</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>13646.24</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>11909.988</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>15168.533</v>
+      </c>
+      <c r="F6" s="2" t="n">
+        <v>35800.819</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <f aca="false">AVERAGE(B6:F6)</f>
+        <v>21403.8092</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <f aca="false">MAX(B6:F6)</f>
+        <v>35800.819</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">MIN(B6:F6)</f>
+        <v>11909.988</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>-0.423</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>-0.012</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>0.027</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>-0.049</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <f aca="false">AVERAGE(B7:F7)</f>
+        <v>-0.0774</v>
+      </c>
+      <c r="H7" s="3" t="n">
+        <f aca="false">MAX(B7:F7)</f>
+        <v>0.07</v>
+      </c>
+      <c r="I7" s="3" t="n">
+        <f aca="false">MIN(B7:F7)</f>
+        <v>-0.423</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>19489.773</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>15673.828</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>11051.153</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>10210.069</v>
+      </c>
+      <c r="F8" s="2" t="n">
+        <v>16742.907</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <f aca="false">AVERAGE(B8:F8)</f>
+        <v>14633.546</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">MAX(B8:F8)</f>
+        <v>19489.773</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">MIN(B8:F8)</f>
+        <v>10210.069</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>20324.703</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>9852.905</v>
+      </c>
+      <c r="D9" s="2" t="n">
+        <v>9407.564</v>
+      </c>
+      <c r="E9" s="2" t="n">
+        <v>11376.4</v>
+      </c>
+      <c r="F9" s="2" t="n">
+        <v>13575.077</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <f aca="false">AVERAGE(B9:F9)</f>
+        <v>12907.3298</v>
+      </c>
+      <c r="H9" s="0" t="n">
+        <f aca="false">MAX(B9:F9)</f>
+        <v>20324.703</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">MIN(B9:F9)</f>
+        <v>9407.564</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="n">
+        <v>-0.043</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>0.371</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0.149</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>-0.114</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>0.189</v>
+      </c>
+      <c r="G10" s="3" t="n">
+        <f aca="false">AVERAGE(B10:F10)</f>
+        <v>0.1104</v>
+      </c>
+      <c r="H10" s="3" t="n">
+        <f aca="false">MAX(B10:F10)</f>
+        <v>0.371</v>
+      </c>
+      <c r="I10" s="3" t="n">
+        <f aca="false">MIN(B10:F10)</f>
+        <v>-0.114</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>120906.532</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>7491.171</v>
+      </c>
+      <c r="D14" s="2" t="n">
+        <v>46110.674</v>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>20431.929</v>
+      </c>
+      <c r="F14" s="2" t="n">
+        <v>36392.609</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <f aca="false">AVERAGE(B14:F14)</f>
+        <v>46266.583</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <f aca="false">MAX(B14:F14)</f>
+        <v>120906.532</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <f aca="false">MIN(B14:F14)</f>
+        <v>7491.171</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>121308.512</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>8977.952</v>
+      </c>
+      <c r="D15" s="2" t="n">
+        <v>42351.768</v>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>22338.152</v>
+      </c>
+      <c r="F15" s="2" t="n">
+        <v>36832.793</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <f aca="false">AVERAGE(B15:F15)</f>
+        <v>46361.8354</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <f aca="false">MAX(B15:F15)</f>
+        <v>121308.512</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <f aca="false">MIN(B15:F15)</f>
+        <v>8977.952</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3" t="n">
+        <v>-0.003</v>
+      </c>
+      <c r="C16" s="4" t="n">
+        <v>-0.198</v>
+      </c>
+      <c r="D16" s="3" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="E16" s="3" t="n">
+        <f aca="false">-0.093</f>
+        <v>-0.093</v>
+      </c>
+      <c r="F16" s="3" t="n">
+        <v>-0.012</v>
+      </c>
+      <c r="G16" s="3" t="n">
+        <f aca="false">AVERAGE(B16:F16)</f>
+        <v>-0.0448</v>
+      </c>
+      <c r="H16" s="3" t="n">
+        <f aca="false">MAX(B16:F16)</f>
+        <v>0.082</v>
+      </c>
+      <c r="I16" s="3" t="n">
+        <f aca="false">MIN(B16:F16)</f>
+        <v>-0.198</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>87365.054</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>4787.118</v>
+      </c>
+      <c r="D17" s="2" t="n">
+        <v>25932.182</v>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>13412.84</v>
+      </c>
+      <c r="F17" s="2" t="n">
+        <v>21954.762</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <f aca="false">AVERAGE(B17:F17)</f>
+        <v>30690.3912</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <f aca="false">MAX(B17:F17)</f>
+        <v>87365.054</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <f aca="false">MIN(B17:F17)</f>
+        <v>4787.118</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>91345.057</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>3858.442</v>
+      </c>
+      <c r="D18" s="2" t="n">
+        <v>30197.259</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>12206.572</v>
+      </c>
+      <c r="F18" s="2" t="n">
+        <v>23126.083</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <f aca="false">AVERAGE(B18:F18)</f>
+        <v>32146.6826</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <f aca="false">MAX(B18:F18)</f>
+        <v>91345.057</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <f aca="false">MIN(B18:F18)</f>
+        <v>3858.442</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="3" t="n">
+        <v>-0.046</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>0.194</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>-0.164</v>
+      </c>
+      <c r="E19" s="3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="F19" s="3" t="n">
+        <v>-0.053</v>
+      </c>
+      <c r="G19" s="3" t="n">
+        <f aca="false">AVERAGE(B19:F19)</f>
+        <v>0.0042</v>
+      </c>
+      <c r="H19" s="3" t="n">
+        <f aca="false">MAX(B19:F19)</f>
+        <v>0.194</v>
+      </c>
+      <c r="I19" s="3" t="n">
+        <f aca="false">MIN(B19:F19)</f>
+        <v>-0.164</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>33541.478</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>2704.053</v>
+      </c>
+      <c r="D20" s="2" t="n">
+        <v>20178.492</v>
+      </c>
+      <c r="E20" s="2" t="n">
+        <v>7019.09</v>
+      </c>
+      <c r="F20" s="2" t="n">
+        <v>14437.847</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">AVERAGE(B20:F20)</f>
+        <v>15576.192</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">MAX(B20:F20)</f>
+        <v>33541.478</v>
+      </c>
+      <c r="I20" s="0" t="n">
+        <f aca="false">MIN(B20:F20)</f>
+        <v>2704.053</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>29963.455</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>5119.51</v>
+      </c>
+      <c r="D21" s="2" t="n">
+        <v>12154.509</v>
+      </c>
+      <c r="E21" s="2" t="n">
+        <v>10131.579</v>
+      </c>
+      <c r="F21" s="2" t="n">
+        <v>13706.709</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">AVERAGE(B21:F21)</f>
+        <v>14215.1524</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">MAX(B21:F21)</f>
+        <v>29963.455</v>
+      </c>
+      <c r="I21" s="0" t="n">
+        <f aca="false">MIN(B21:F21)</f>
+        <v>5119.51</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="4" t="n">
+        <v>0.107</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>-0.893</v>
+      </c>
+      <c r="D22" s="4" t="n">
+        <v>0.398</v>
+      </c>
+      <c r="E22" s="4" t="n">
+        <v>-0.443</v>
+      </c>
+      <c r="F22" s="3" t="n">
+        <v>0.051</v>
+      </c>
+      <c r="G22" s="3" t="n">
+        <f aca="false">AVERAGE(B22:F22)</f>
+        <v>-0.156</v>
+      </c>
+      <c r="H22" s="3" t="n">
+        <f aca="false">MAX(B22:F22)</f>
+        <v>0.398</v>
+      </c>
+      <c r="I22" s="3" t="n">
+        <f aca="false">MIN(B22:F22)</f>
+        <v>-0.893</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>45589.83</v>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>49072.841</v>
+      </c>
+      <c r="D26" s="2" t="n">
+        <v>26973.267</v>
+      </c>
+      <c r="E26" s="2" t="n">
+        <v>42684.858</v>
+      </c>
+      <c r="F26" s="2" t="n">
+        <v>28945.423</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <v>45716.501</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">AVERAGE(B26:G26)</f>
+        <v>39830.4533333333</v>
+      </c>
+      <c r="I26" s="0" t="n">
+        <f aca="false">MAX(B26:G26)</f>
+        <v>49072.841</v>
+      </c>
+      <c r="J26" s="0" t="n">
+        <f aca="false">MIN(B26:G26)</f>
+        <v>26973.267</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>45878.093</v>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>48800.236</v>
+      </c>
+      <c r="D27" s="2" t="n">
+        <v>26687.622</v>
+      </c>
+      <c r="E27" s="2" t="n">
+        <v>43388.823</v>
+      </c>
+      <c r="F27" s="2" t="n">
+        <v>28303.83</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>45305.656</v>
+      </c>
+      <c r="H27" s="0" t="n">
+        <f aca="false">AVERAGE(B27:G27)</f>
+        <v>39727.3766666667</v>
+      </c>
+      <c r="I27" s="0" t="n">
+        <f aca="false">MAX(B27:G27)</f>
+        <v>48800.236</v>
+      </c>
+      <c r="J27" s="0" t="n">
+        <f aca="false">MIN(B27:G27)</f>
+        <v>26687.622</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>-0.006</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="D28" s="3" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="E28" s="3" t="n">
+        <v>-0.016</v>
+      </c>
+      <c r="F28" s="3" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="G28" s="3" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="H28" s="3" t="n">
+        <f aca="false">AVERAGE(B28:G28)</f>
+        <v>0.00433333333333333</v>
+      </c>
+      <c r="I28" s="3" t="n">
+        <f aca="false">MAX(B28:G28)</f>
+        <v>0.022</v>
+      </c>
+      <c r="J28" s="3" t="n">
+        <f aca="false">MIN(B28:G28)</f>
+        <v>-0.016</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>38128.295</v>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>39803.483</v>
+      </c>
+      <c r="D29" s="2" t="n">
+        <v>21814.27</v>
+      </c>
+      <c r="E29" s="2" t="n">
+        <v>35908.137</v>
+      </c>
+      <c r="F29" s="2" t="n">
+        <v>23283.182</v>
+      </c>
+      <c r="G29" s="0" t="n">
+        <v>36377.436</v>
+      </c>
+      <c r="H29" s="0" t="n">
+        <f aca="false">AVERAGE(B29:G29)</f>
+        <v>32552.4671666667</v>
+      </c>
+      <c r="I29" s="0" t="n">
+        <f aca="false">MAX(B29:G29)</f>
+        <v>39803.483</v>
+      </c>
+      <c r="J29" s="0" t="n">
+        <f aca="false">MIN(B29:G29)</f>
+        <v>21814.27</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>38986.887</v>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>42240.479</v>
+      </c>
+      <c r="D30" s="2" t="n">
+        <v>22363.586</v>
+      </c>
+      <c r="E30" s="2" t="n">
+        <v>36310.16</v>
+      </c>
+      <c r="F30" s="2" t="n">
+        <v>24340.704</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <v>37970.228</v>
+      </c>
+      <c r="H30" s="0" t="n">
+        <f aca="false">AVERAGE(B30:G30)</f>
+        <v>33702.0073333333</v>
+      </c>
+      <c r="I30" s="0" t="n">
+        <f aca="false">MAX(B30:G30)</f>
+        <v>42240.479</v>
+      </c>
+      <c r="J30" s="0" t="n">
+        <f aca="false">MIN(B30:G30)</f>
+        <v>22363.586</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" s="3" t="n">
+        <v>-0.023</v>
+      </c>
+      <c r="C31" s="3" t="n">
+        <f aca="false">-0.061</f>
+        <v>-0.061</v>
+      </c>
+      <c r="D31" s="3" t="n">
+        <v>-0.025</v>
+      </c>
+      <c r="E31" s="3" t="n">
+        <v>-0.011</v>
+      </c>
+      <c r="F31" s="3" t="n">
+        <v>-0.045</v>
+      </c>
+      <c r="G31" s="3" t="n">
+        <v>-0.044</v>
+      </c>
+      <c r="H31" s="3" t="n">
+        <f aca="false">AVERAGE(B31:G31)</f>
+        <v>-0.0348333333333333</v>
+      </c>
+      <c r="I31" s="3" t="n">
+        <f aca="false">MAX(B31:G31)</f>
+        <v>-0.011</v>
+      </c>
+      <c r="J31" s="3" t="n">
+        <f aca="false">MIN(B31:G31)</f>
+        <v>-0.061</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>7461.535</v>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>9269.358</v>
+      </c>
+      <c r="D32" s="2" t="n">
+        <v>5158.997</v>
+      </c>
+      <c r="E32" s="2" t="n">
+        <v>6776.721</v>
+      </c>
+      <c r="F32" s="2" t="n">
+        <v>5662.241</v>
+      </c>
+      <c r="G32" s="0" t="n">
+        <v>9339.065</v>
+      </c>
+      <c r="H32" s="0" t="n">
+        <f aca="false">AVERAGE(B32:G32)</f>
+        <v>7277.98616666667</v>
+      </c>
+      <c r="I32" s="0" t="n">
+        <f aca="false">MAX(B32:G32)</f>
+        <v>9339.065</v>
+      </c>
+      <c r="J32" s="0" t="n">
+        <f aca="false">MIN(B32:G32)</f>
+        <v>5158.997</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>6891.207</v>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>6559.757</v>
+      </c>
+      <c r="D33" s="2" t="n">
+        <v>4324.036</v>
+      </c>
+      <c r="E33" s="2" t="n">
+        <v>7078.662</v>
+      </c>
+      <c r="F33" s="2" t="n">
+        <v>3963.126</v>
+      </c>
+      <c r="G33" s="0" t="n">
+        <v>7335.428</v>
+      </c>
+      <c r="H33" s="0" t="n">
+        <f aca="false">AVERAGE(B33:G33)</f>
+        <v>6025.36933333333</v>
+      </c>
+      <c r="I33" s="0" t="n">
+        <f aca="false">MAX(B33:G33)</f>
+        <v>7335.428</v>
+      </c>
+      <c r="J33" s="0" t="n">
+        <f aca="false">MIN(B33:G33)</f>
+        <v>3963.126</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="3" t="n">
+        <v>0.076</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>0.292</v>
+      </c>
+      <c r="D34" s="4" t="n">
+        <v>0.162</v>
+      </c>
+      <c r="E34" s="3" t="n">
+        <v>-0.045</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <v>0.215</v>
+      </c>
+      <c r="H34" s="3" t="n">
+        <f aca="false">AVERAGE(B34:G34)</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="I34" s="3" t="n">
+        <f aca="false">MAX(B34:G34)</f>
+        <v>0.3</v>
+      </c>
+      <c r="J34" s="3" t="n">
+        <f aca="false">MIN(B34:G34)</f>
+        <v>-0.045</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>152785.42</v>
+      </c>
+      <c r="C38" s="2" t="n">
+        <v>22957.563</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <f aca="false">AVERAGE(B38:C38)</f>
+        <v>87871.4915</v>
+      </c>
+      <c r="E38" s="0" t="n">
+        <f aca="false">MAX(B38:C38)</f>
+        <v>152785.42</v>
+      </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">MIN(B38:C38)</f>
+        <v>22957.563</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>151229.024</v>
+      </c>
+      <c r="C39" s="5" t="n">
+        <v>22390.008</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <f aca="false">AVERAGE(B39:C39)</f>
+        <v>86809.516</v>
+      </c>
+      <c r="E39" s="0" t="n">
+        <f aca="false">MAX(B39:C39)</f>
+        <v>151229.024</v>
+      </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">MIN(B39:C39)</f>
+        <v>22390.008</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="3" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C40" s="3" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="D40" s="3" t="n">
+        <f aca="false">AVERAGE(B40:C40)</f>
+        <v>0.0175</v>
+      </c>
+      <c r="E40" s="3" t="n">
+        <f aca="false">MAX(B40:C40)</f>
+        <v>0.025</v>
+      </c>
+      <c r="F40" s="3" t="n">
+        <f aca="false">MIN(B40:C40)</f>
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>112816.93</v>
+      </c>
+      <c r="C41" s="2" t="n">
+        <v>11912.942</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <f aca="false">AVERAGE(B41:C41)</f>
+        <v>62364.936</v>
+      </c>
+      <c r="E41" s="0" t="n">
+        <f aca="false">MAX(B41:C41)</f>
+        <v>112816.93</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">MIN(B41:C41)</f>
+        <v>11912.942</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>112981.439</v>
+      </c>
+      <c r="C42" s="2" t="n">
+        <v>12320.28</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <f aca="false">AVERAGE(B42:C42)</f>
+        <v>62650.8595</v>
+      </c>
+      <c r="E42" s="0" t="n">
+        <f aca="false">MAX(B42:C42)</f>
+        <v>112981.439</v>
+      </c>
+      <c r="F42" s="0" t="n">
+        <f aca="false">MIN(B42:C42)</f>
+        <v>12320.28</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="3" t="n">
+        <v>-0.001</v>
+      </c>
+      <c r="C43" s="3" t="n">
+        <v>-0.034</v>
+      </c>
+      <c r="D43" s="3" t="n">
+        <f aca="false">AVERAGE(B43:C43)</f>
+        <v>-0.0175</v>
+      </c>
+      <c r="E43" s="3" t="n">
+        <f aca="false">MAX(B43:C43)</f>
+        <v>-0.001</v>
+      </c>
+      <c r="F43" s="3" t="n">
+        <f aca="false">MIN(B43:C43)</f>
+        <v>-0.034</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="2" t="n">
+        <v>39968.491</v>
+      </c>
+      <c r="C44" s="2" t="n">
+        <v>11044.621</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <f aca="false">AVERAGE(B44:C44)</f>
+        <v>25506.556</v>
+      </c>
+      <c r="E44" s="0" t="n">
+        <f aca="false">MAX(B44:C44)</f>
+        <v>39968.491</v>
+      </c>
+      <c r="F44" s="0" t="n">
+        <f aca="false">MIN(B44:C44)</f>
+        <v>11044.621</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>38247.585</v>
+      </c>
+      <c r="C45" s="2" t="n">
+        <v>10069.728</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <f aca="false">AVERAGE(B45:C45)</f>
+        <v>24158.6565</v>
+      </c>
+      <c r="E45" s="0" t="n">
+        <f aca="false">MAX(B45:C45)</f>
+        <v>38247.585</v>
+      </c>
+      <c r="F45" s="0" t="n">
+        <f aca="false">MIN(B45:C45)</f>
+        <v>10069.728</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="3" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="C46" s="3" t="n">
+        <v>0.088</v>
+      </c>
+      <c r="D46" s="3" t="n">
+        <f aca="false">AVERAGE(B46:C46)</f>
+        <v>0.0655</v>
+      </c>
+      <c r="E46" s="3" t="n">
+        <f aca="false">MAX(B46:C46)</f>
+        <v>0.088</v>
+      </c>
+      <c r="F46" s="3" t="n">
+        <f aca="false">MIN(B46:C46)</f>
+        <v>0.043</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>